<commit_message>
Corrected errors in calculating liquid hydrocarbon energy demand
</commit_message>
<xml_diff>
--- a/InputData/indst/BPoIFUfE/BAU Proportion of Industrial Fuel Used for Energy.xlsx
+++ b/InputData/indst/BPoIFUfE/BAU Proportion of Industrial Fuel Used for Energy.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS India 2.1 - Input Data Revisions_17Mar2020\BPoIFUfE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\indst\BPoIFUfE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A4944A-9242-46ED-A618-74F6AE90335E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -165,7 +164,7 @@
     <definedName name="XIV.d.AreaRatio">[1]Control!$E$63</definedName>
     <definedName name="XIV.e.Area">[1]Control!$E$64</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -889,7 +888,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="###0_);\(###0\)"/>
@@ -1694,76 +1693,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1798,6 +1727,76 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3496,24 +3495,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="2" max="2" width="58.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3521,139 +3520,139 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="3">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" s="3">
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -3661,92 +3660,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V201"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" style="105" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="105" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="105" customWidth="1"/>
+    <col min="1" max="1" width="33.59765625" style="105" customWidth="1"/>
+    <col min="2" max="2" width="32.59765625" style="105" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.59765625" style="105" customWidth="1"/>
     <col min="4" max="4" width="22" style="105" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="105" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="105" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="105" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="105" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="105"/>
-    <col min="12" max="12" width="34.140625" style="105" customWidth="1"/>
-    <col min="13" max="13" width="32.5703125" style="105" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="105" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="105" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" style="105" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" style="105" customWidth="1"/>
+    <col min="5" max="5" width="22.265625" style="105" customWidth="1"/>
+    <col min="6" max="6" width="16.73046875" style="105" customWidth="1"/>
+    <col min="7" max="7" width="10.265625" style="105" customWidth="1"/>
+    <col min="8" max="8" width="9.86328125" style="105" customWidth="1"/>
+    <col min="9" max="9" width="9.1328125" style="105"/>
+    <col min="12" max="12" width="34.1328125" style="105" customWidth="1"/>
+    <col min="13" max="13" width="32.59765625" style="105" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.1328125" style="105" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.59765625" style="105" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.265625" style="105" customWidth="1"/>
+    <col min="17" max="17" width="10.73046875" style="105" customWidth="1"/>
+    <col min="18" max="18" width="8.73046875" style="105" customWidth="1"/>
     <col min="19" max="19" width="10" style="105" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="105"/>
-    <col min="22" max="22" width="21.42578125" customWidth="1"/>
+    <col min="20" max="20" width="9.1328125" style="105"/>
+    <col min="22" max="22" width="21.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+    <row r="1" spans="1:22" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="128" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="109"/>
-      <c r="L1" s="107" t="s">
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="130"/>
+      <c r="L1" s="128" t="s">
         <v>124</v>
       </c>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="109"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
+      <c r="P1" s="129"/>
+      <c r="Q1" s="129"/>
+      <c r="R1" s="129"/>
+      <c r="S1" s="129"/>
+      <c r="T1" s="130"/>
       <c r="V1" s="35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A2" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="112"/>
-      <c r="L2" s="113" t="s">
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="135"/>
+      <c r="L2" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="112"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="114" t="s">
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="135"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A3" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="115"/>
+      <c r="B3" s="123"/>
       <c r="C3" s="36" t="s">
         <v>126</v>
       </c>
@@ -3768,10 +3767,10 @@
       <c r="I3" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="114" t="s">
+      <c r="L3" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="M3" s="115"/>
+      <c r="M3" s="123"/>
       <c r="N3" s="36" t="s">
         <v>126</v>
       </c>
@@ -3794,11 +3793,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="116">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A4" s="124">
         <v>-1</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="125"/>
       <c r="C4" s="38">
         <v>-2</v>
       </c>
@@ -3820,10 +3819,10 @@
       <c r="I4" s="39">
         <v>-8</v>
       </c>
-      <c r="L4" s="116">
+      <c r="L4" s="124">
         <v>-1</v>
       </c>
-      <c r="M4" s="117"/>
+      <c r="M4" s="125"/>
       <c r="N4" s="38">
         <v>-2</v>
       </c>
@@ -3846,7 +3845,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="40">
         <v>1</v>
       </c>
@@ -3902,7 +3901,7 @@
         <v>912611422608631.25</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="103">
         <v>2</v>
       </c>
@@ -3961,7 +3960,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="103">
         <v>3</v>
       </c>
@@ -4017,7 +4016,7 @@
         <v>8292635523470.4805</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" s="46" t="s">
         <v>134</v>
       </c>
@@ -4073,7 +4072,7 @@
         <v>8262142947058</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" s="46" t="s">
         <v>136</v>
       </c>
@@ -4129,7 +4128,7 @@
         <v>30492576412.48</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" s="103">
         <v>4</v>
       </c>
@@ -4185,7 +4184,7 @@
         <v>56052530170</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="103">
         <v>5</v>
       </c>
@@ -4244,7 +4243,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" s="103">
         <v>6</v>
       </c>
@@ -4303,7 +4302,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" s="103">
         <v>7</v>
       </c>
@@ -4359,7 +4358,7 @@
         <v>9163019211950.2383</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" s="46" t="s">
         <v>134</v>
       </c>
@@ -4418,7 +4417,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15" s="46" t="s">
         <v>136</v>
       </c>
@@ -4477,7 +4476,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16" s="46" t="s">
         <v>142</v>
       </c>
@@ -4536,7 +4535,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" s="46" t="s">
         <v>144</v>
       </c>
@@ -4595,7 +4594,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18" s="46" t="s">
         <v>146</v>
       </c>
@@ -4654,7 +4653,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" s="46" t="s">
         <v>148</v>
       </c>
@@ -4713,7 +4712,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" s="46" t="s">
         <v>150</v>
       </c>
@@ -4772,7 +4771,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" s="103">
         <v>8</v>
       </c>
@@ -4831,7 +4830,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" s="103">
         <v>9</v>
       </c>
@@ -4890,7 +4889,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A23" s="51"/>
       <c r="B23" s="52" t="s">
         <v>155</v>
@@ -4943,7 +4942,7 @@
         <v>1030314561241769.5</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A24" s="57">
         <v>10</v>
       </c>
@@ -4999,11 +4998,11 @@
         <v>16452538655498.398</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="118" t="s">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A25" s="143" t="s">
         <v>157</v>
       </c>
-      <c r="B25" s="119"/>
+      <c r="B25" s="144"/>
       <c r="C25" s="61">
         <v>15349.7</v>
       </c>
@@ -5025,10 +5024,10 @@
       <c r="I25" s="63">
         <v>23343.439999999999</v>
       </c>
-      <c r="L25" s="118" t="s">
+      <c r="L25" s="143" t="s">
         <v>157</v>
       </c>
-      <c r="M25" s="119"/>
+      <c r="M25" s="144"/>
       <c r="N25" s="64">
         <v>688311617880359.25</v>
       </c>
@@ -5051,7 +5050,7 @@
         <v>1046767099897267.8</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A26" s="14" t="s">
         <v>158</v>
       </c>
@@ -5075,7 +5074,7 @@
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A27" s="14" t="s">
         <v>159</v>
       </c>
@@ -5099,7 +5098,7 @@
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.45">
       <c r="C28" s="66"/>
       <c r="D28" s="66"/>
       <c r="E28" s="66"/>
@@ -5108,59 +5107,59 @@
       <c r="H28" s="66"/>
       <c r="I28" s="66"/>
     </row>
-    <row r="29" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="107" t="s">
+    <row r="29" spans="1:22" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A29" s="128" t="s">
         <v>160</v>
       </c>
-      <c r="B29" s="108"/>
-      <c r="C29" s="108"/>
-      <c r="D29" s="108"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="108"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="109"/>
-      <c r="L29" s="107" t="s">
+      <c r="B29" s="129"/>
+      <c r="C29" s="129"/>
+      <c r="D29" s="129"/>
+      <c r="E29" s="129"/>
+      <c r="F29" s="129"/>
+      <c r="G29" s="129"/>
+      <c r="H29" s="129"/>
+      <c r="I29" s="130"/>
+      <c r="L29" s="128" t="s">
         <v>160</v>
       </c>
-      <c r="M29" s="108"/>
-      <c r="N29" s="108"/>
-      <c r="O29" s="108"/>
-      <c r="P29" s="108"/>
-      <c r="Q29" s="108"/>
-      <c r="R29" s="108"/>
-      <c r="S29" s="108"/>
-      <c r="T29" s="109"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="110" t="s">
+      <c r="M29" s="129"/>
+      <c r="N29" s="129"/>
+      <c r="O29" s="129"/>
+      <c r="P29" s="129"/>
+      <c r="Q29" s="129"/>
+      <c r="R29" s="129"/>
+      <c r="S29" s="129"/>
+      <c r="T29" s="130"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A30" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B30" s="111"/>
-      <c r="C30" s="111"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="111"/>
-      <c r="F30" s="111"/>
-      <c r="G30" s="111"/>
-      <c r="H30" s="111"/>
-      <c r="I30" s="112"/>
-      <c r="L30" s="113" t="s">
+      <c r="B30" s="134"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="134"/>
+      <c r="G30" s="134"/>
+      <c r="H30" s="134"/>
+      <c r="I30" s="135"/>
+      <c r="L30" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="M30" s="111"/>
-      <c r="N30" s="111"/>
-      <c r="O30" s="111"/>
-      <c r="P30" s="111"/>
-      <c r="Q30" s="111"/>
-      <c r="R30" s="111"/>
-      <c r="S30" s="111"/>
-      <c r="T30" s="112"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="114" t="s">
+      <c r="M30" s="134"/>
+      <c r="N30" s="134"/>
+      <c r="O30" s="134"/>
+      <c r="P30" s="134"/>
+      <c r="Q30" s="134"/>
+      <c r="R30" s="134"/>
+      <c r="S30" s="134"/>
+      <c r="T30" s="135"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A31" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="115"/>
+      <c r="B31" s="123"/>
       <c r="C31" s="36" t="s">
         <v>126</v>
       </c>
@@ -5182,10 +5181,10 @@
       <c r="I31" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="L31" s="114" t="s">
+      <c r="L31" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="M31" s="115"/>
+      <c r="M31" s="123"/>
       <c r="N31" s="36" t="s">
         <v>126</v>
       </c>
@@ -5208,11 +5207,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="116">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A32" s="124">
         <v>-1</v>
       </c>
-      <c r="B32" s="117"/>
+      <c r="B32" s="125"/>
       <c r="C32" s="38">
         <v>-2</v>
       </c>
@@ -5234,10 +5233,10 @@
       <c r="I32" s="38">
         <v>-8</v>
       </c>
-      <c r="L32" s="116">
+      <c r="L32" s="124">
         <v>-1</v>
       </c>
-      <c r="M32" s="117"/>
+      <c r="M32" s="125"/>
       <c r="N32" s="38">
         <v>-2</v>
       </c>
@@ -5260,7 +5259,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A33" s="67">
         <v>1</v>
       </c>
@@ -5319,7 +5318,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A34" s="68">
         <v>2</v>
       </c>
@@ -5378,7 +5377,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A35" s="68">
         <v>3</v>
       </c>
@@ -5434,7 +5433,7 @@
         <v>2851762255655.04</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A36" s="68">
         <v>4</v>
       </c>
@@ -5493,7 +5492,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A37" s="68">
         <v>5</v>
       </c>
@@ -5552,7 +5551,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A38" s="51"/>
       <c r="B38" s="52" t="s">
         <v>155</v>
@@ -5604,7 +5603,7 @@
         <v>464646101599330.56</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A39" s="57">
         <v>6</v>
       </c>
@@ -5660,11 +5659,11 @@
         <v>73175088032504.656</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="118" t="s">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A40" s="143" t="s">
         <v>157</v>
       </c>
-      <c r="B40" s="119"/>
+      <c r="B40" s="144"/>
       <c r="C40" s="61">
         <v>11221.5</v>
       </c>
@@ -5686,10 +5685,10 @@
       <c r="I40" s="61">
         <v>12548.95</v>
       </c>
-      <c r="L40" s="118" t="s">
+      <c r="L40" s="143" t="s">
         <v>157</v>
       </c>
-      <c r="M40" s="119"/>
+      <c r="M40" s="144"/>
       <c r="N40" s="64">
         <v>480929518362384.13</v>
       </c>
@@ -5712,7 +5711,7 @@
         <v>537821189631835.31</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A41" s="14" t="s">
         <v>166</v>
       </c>
@@ -5736,7 +5735,7 @@
       <c r="S41" s="15"/>
       <c r="T41" s="15"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A42" s="14" t="s">
         <v>159</v>
       </c>
@@ -5760,59 +5759,59 @@
       <c r="S42" s="15"/>
       <c r="T42" s="15"/>
     </row>
-    <row r="44" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="107" t="s">
+    <row r="44" spans="1:22" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A44" s="128" t="s">
         <v>167</v>
       </c>
-      <c r="B44" s="108"/>
-      <c r="C44" s="108"/>
-      <c r="D44" s="108"/>
-      <c r="E44" s="108"/>
-      <c r="F44" s="108"/>
-      <c r="G44" s="108"/>
-      <c r="H44" s="108"/>
-      <c r="I44" s="109"/>
-      <c r="L44" s="107" t="s">
+      <c r="B44" s="129"/>
+      <c r="C44" s="129"/>
+      <c r="D44" s="129"/>
+      <c r="E44" s="129"/>
+      <c r="F44" s="129"/>
+      <c r="G44" s="129"/>
+      <c r="H44" s="129"/>
+      <c r="I44" s="130"/>
+      <c r="L44" s="128" t="s">
         <v>167</v>
       </c>
-      <c r="M44" s="108"/>
-      <c r="N44" s="108"/>
-      <c r="O44" s="108"/>
-      <c r="P44" s="108"/>
-      <c r="Q44" s="108"/>
-      <c r="R44" s="108"/>
-      <c r="S44" s="108"/>
-      <c r="T44" s="109"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45" s="110" t="s">
+      <c r="M44" s="129"/>
+      <c r="N44" s="129"/>
+      <c r="O44" s="129"/>
+      <c r="P44" s="129"/>
+      <c r="Q44" s="129"/>
+      <c r="R44" s="129"/>
+      <c r="S44" s="129"/>
+      <c r="T44" s="130"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A45" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="111"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="112"/>
-      <c r="L45" s="113" t="s">
+      <c r="B45" s="134"/>
+      <c r="C45" s="134"/>
+      <c r="D45" s="134"/>
+      <c r="E45" s="134"/>
+      <c r="F45" s="134"/>
+      <c r="G45" s="134"/>
+      <c r="H45" s="134"/>
+      <c r="I45" s="135"/>
+      <c r="L45" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="M45" s="111"/>
-      <c r="N45" s="111"/>
-      <c r="O45" s="111"/>
-      <c r="P45" s="111"/>
-      <c r="Q45" s="111"/>
-      <c r="R45" s="111"/>
-      <c r="S45" s="111"/>
-      <c r="T45" s="112"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="114" t="s">
+      <c r="M45" s="134"/>
+      <c r="N45" s="134"/>
+      <c r="O45" s="134"/>
+      <c r="P45" s="134"/>
+      <c r="Q45" s="134"/>
+      <c r="R45" s="134"/>
+      <c r="S45" s="134"/>
+      <c r="T45" s="135"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A46" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="115"/>
+      <c r="B46" s="123"/>
       <c r="C46" s="36" t="s">
         <v>126</v>
       </c>
@@ -5834,10 +5833,10 @@
       <c r="I46" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="L46" s="114" t="s">
+      <c r="L46" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="M46" s="115"/>
+      <c r="M46" s="123"/>
       <c r="N46" s="36" t="s">
         <v>126</v>
       </c>
@@ -5860,11 +5859,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="116">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A47" s="124">
         <v>-1</v>
       </c>
-      <c r="B47" s="117"/>
+      <c r="B47" s="125"/>
       <c r="C47" s="38">
         <v>-2</v>
       </c>
@@ -5886,10 +5885,10 @@
       <c r="I47" s="38">
         <v>-8</v>
       </c>
-      <c r="L47" s="116">
+      <c r="L47" s="124">
         <v>-1</v>
       </c>
-      <c r="M47" s="117"/>
+      <c r="M47" s="125"/>
       <c r="N47" s="38">
         <v>-2</v>
       </c>
@@ -5912,7 +5911,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A48" s="40">
         <v>1</v>
       </c>
@@ -5968,7 +5967,7 @@
         <v>247055780764086.88</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A49" s="71" t="s">
         <v>134</v>
       </c>
@@ -6024,7 +6023,7 @@
         <v>112022562920551.92</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A50" s="46" t="s">
         <v>136</v>
       </c>
@@ -6080,7 +6079,7 @@
         <v>113769770882.04001</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A51" s="46" t="s">
         <v>142</v>
       </c>
@@ -6136,7 +6135,7 @@
         <v>26582697151723.445</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A52" s="46" t="s">
         <v>144</v>
       </c>
@@ -6192,7 +6191,7 @@
         <v>108337161642123.97</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A53" s="103">
         <v>2</v>
       </c>
@@ -6251,7 +6250,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A54" s="103">
         <v>3</v>
       </c>
@@ -6307,7 +6306,7 @@
         <v>8654306289730.9229</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A55" s="103">
         <v>4</v>
       </c>
@@ -6366,7 +6365,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A56" s="103">
         <v>5</v>
       </c>
@@ -6422,7 +6421,7 @@
         <v>46002827392212.609</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A57" s="71" t="s">
         <v>134</v>
       </c>
@@ -6481,7 +6480,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A58" s="46" t="s">
         <v>136</v>
       </c>
@@ -6540,7 +6539,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A59" s="46" t="s">
         <v>142</v>
       </c>
@@ -6599,7 +6598,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A60" s="46" t="s">
         <v>144</v>
       </c>
@@ -6658,7 +6657,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A61" s="46" t="s">
         <v>146</v>
       </c>
@@ -6717,7 +6716,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A62" s="46" t="s">
         <v>148</v>
       </c>
@@ -6776,7 +6775,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A63" s="46" t="s">
         <v>150</v>
       </c>
@@ -6835,7 +6834,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A64" s="46" t="s">
         <v>178</v>
       </c>
@@ -6894,7 +6893,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A65" s="46" t="s">
         <v>180</v>
       </c>
@@ -6953,7 +6952,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A66" s="46" t="s">
         <v>181</v>
       </c>
@@ -7012,7 +7011,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A67" s="46" t="s">
         <v>183</v>
       </c>
@@ -7071,7 +7070,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A68" s="103">
         <v>6</v>
       </c>
@@ -7130,7 +7129,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A69" s="103">
         <v>7</v>
       </c>
@@ -7189,7 +7188,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A70" s="51"/>
       <c r="B70" s="52" t="s">
         <v>184</v>
@@ -7241,8 +7240,8 @@
         <v>3326462579949458</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A71" s="120">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A71" s="131">
         <v>8</v>
       </c>
       <c r="B71" s="58" t="s">
@@ -7269,7 +7268,7 @@
       <c r="I71" s="70">
         <v>82.44</v>
       </c>
-      <c r="L71" s="120">
+      <c r="L71" s="131">
         <v>8</v>
       </c>
       <c r="M71" s="58" t="s">
@@ -7297,8 +7296,8 @@
         <v>3385985527622.8804</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A72" s="121"/>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A72" s="132"/>
       <c r="B72" s="74" t="s">
         <v>157</v>
       </c>
@@ -7323,7 +7322,7 @@
       <c r="I72" s="75">
         <v>81073.210000000006</v>
       </c>
-      <c r="L72" s="121"/>
+      <c r="L72" s="132"/>
       <c r="M72" s="74" t="s">
         <v>157</v>
       </c>
@@ -7349,7 +7348,7 @@
         <v>3329848565477081.5</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A73" s="14" t="s">
         <v>166</v>
       </c>
@@ -7373,7 +7372,7 @@
       <c r="S73" s="15"/>
       <c r="T73" s="15"/>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A74" s="14" t="s">
         <v>159</v>
       </c>
@@ -7397,59 +7396,59 @@
       <c r="S74" s="15"/>
       <c r="T74" s="15"/>
     </row>
-    <row r="76" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="107" t="s">
+    <row r="76" spans="1:22" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A76" s="128" t="s">
         <v>185</v>
       </c>
-      <c r="B76" s="108"/>
-      <c r="C76" s="108"/>
-      <c r="D76" s="108"/>
-      <c r="E76" s="108"/>
-      <c r="F76" s="108"/>
-      <c r="G76" s="108"/>
-      <c r="H76" s="108"/>
-      <c r="I76" s="109"/>
-      <c r="L76" s="107" t="s">
+      <c r="B76" s="129"/>
+      <c r="C76" s="129"/>
+      <c r="D76" s="129"/>
+      <c r="E76" s="129"/>
+      <c r="F76" s="129"/>
+      <c r="G76" s="129"/>
+      <c r="H76" s="129"/>
+      <c r="I76" s="130"/>
+      <c r="L76" s="128" t="s">
         <v>185</v>
       </c>
-      <c r="M76" s="108"/>
-      <c r="N76" s="108"/>
-      <c r="O76" s="108"/>
-      <c r="P76" s="108"/>
-      <c r="Q76" s="108"/>
-      <c r="R76" s="108"/>
-      <c r="S76" s="108"/>
-      <c r="T76" s="109"/>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A77" s="110" t="s">
+      <c r="M76" s="129"/>
+      <c r="N76" s="129"/>
+      <c r="O76" s="129"/>
+      <c r="P76" s="129"/>
+      <c r="Q76" s="129"/>
+      <c r="R76" s="129"/>
+      <c r="S76" s="129"/>
+      <c r="T76" s="130"/>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A77" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B77" s="111"/>
-      <c r="C77" s="111"/>
-      <c r="D77" s="111"/>
-      <c r="E77" s="111"/>
-      <c r="F77" s="111"/>
-      <c r="G77" s="111"/>
-      <c r="H77" s="111"/>
-      <c r="I77" s="112"/>
-      <c r="L77" s="113" t="s">
+      <c r="B77" s="134"/>
+      <c r="C77" s="134"/>
+      <c r="D77" s="134"/>
+      <c r="E77" s="134"/>
+      <c r="F77" s="134"/>
+      <c r="G77" s="134"/>
+      <c r="H77" s="134"/>
+      <c r="I77" s="135"/>
+      <c r="L77" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="M77" s="111"/>
-      <c r="N77" s="111"/>
-      <c r="O77" s="111"/>
-      <c r="P77" s="111"/>
-      <c r="Q77" s="111"/>
-      <c r="R77" s="111"/>
-      <c r="S77" s="111"/>
-      <c r="T77" s="112"/>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A78" s="114" t="s">
+      <c r="M77" s="134"/>
+      <c r="N77" s="134"/>
+      <c r="O77" s="134"/>
+      <c r="P77" s="134"/>
+      <c r="Q77" s="134"/>
+      <c r="R77" s="134"/>
+      <c r="S77" s="134"/>
+      <c r="T77" s="135"/>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A78" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="B78" s="115"/>
+      <c r="B78" s="123"/>
       <c r="C78" s="36" t="s">
         <v>126</v>
       </c>
@@ -7471,10 +7470,10 @@
       <c r="I78" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="L78" s="114" t="s">
+      <c r="L78" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="M78" s="115"/>
+      <c r="M78" s="123"/>
       <c r="N78" s="36" t="s">
         <v>126</v>
       </c>
@@ -7497,11 +7496,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A79" s="116">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A79" s="124">
         <v>-1</v>
       </c>
-      <c r="B79" s="117"/>
+      <c r="B79" s="125"/>
       <c r="C79" s="38">
         <v>-2</v>
       </c>
@@ -7523,10 +7522,10 @@
       <c r="I79" s="38">
         <v>-8</v>
       </c>
-      <c r="L79" s="116">
+      <c r="L79" s="124">
         <v>-1</v>
       </c>
-      <c r="M79" s="117"/>
+      <c r="M79" s="125"/>
       <c r="N79" s="38">
         <v>-2</v>
       </c>
@@ -7549,31 +7548,31 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A80" s="122" t="s">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A80" s="137" t="s">
         <v>186</v>
       </c>
-      <c r="B80" s="123"/>
-      <c r="C80" s="123"/>
-      <c r="D80" s="123"/>
-      <c r="E80" s="123"/>
-      <c r="F80" s="123"/>
-      <c r="G80" s="123"/>
-      <c r="H80" s="123"/>
-      <c r="I80" s="124"/>
-      <c r="L80" s="125" t="s">
+      <c r="B80" s="138"/>
+      <c r="C80" s="138"/>
+      <c r="D80" s="138"/>
+      <c r="E80" s="138"/>
+      <c r="F80" s="138"/>
+      <c r="G80" s="138"/>
+      <c r="H80" s="138"/>
+      <c r="I80" s="139"/>
+      <c r="L80" s="140" t="s">
         <v>186</v>
       </c>
-      <c r="M80" s="126"/>
-      <c r="N80" s="126"/>
-      <c r="O80" s="126"/>
-      <c r="P80" s="126"/>
-      <c r="Q80" s="126"/>
-      <c r="R80" s="126"/>
-      <c r="S80" s="126"/>
-      <c r="T80" s="127"/>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="M80" s="141"/>
+      <c r="N80" s="141"/>
+      <c r="O80" s="141"/>
+      <c r="P80" s="141"/>
+      <c r="Q80" s="141"/>
+      <c r="R80" s="141"/>
+      <c r="S80" s="141"/>
+      <c r="T80" s="142"/>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A81" s="40">
         <v>1</v>
       </c>
@@ -7629,7 +7628,7 @@
         <v>324799114290.56006</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A82" s="71" t="s">
         <v>134</v>
       </c>
@@ -7685,7 +7684,7 @@
         <v>124637017173.76001</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A83" s="46" t="s">
         <v>136</v>
       </c>
@@ -7741,7 +7740,7 @@
         <v>178701418663.04004</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A84" s="46" t="s">
         <v>142</v>
       </c>
@@ -7797,7 +7796,7 @@
         <v>21047973098.880001</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A85" s="103">
         <v>2</v>
       </c>
@@ -7856,7 +7855,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A86" s="103">
         <v>3</v>
       </c>
@@ -7912,7 +7911,7 @@
         <v>5884765655233.9199</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A87" s="103">
         <v>4</v>
       </c>
@@ -7971,7 +7970,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A88" s="103">
         <v>5</v>
       </c>
@@ -8027,7 +8026,7 @@
         <v>5982164118985.6006</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A89" s="71" t="s">
         <v>134</v>
       </c>
@@ -8086,7 +8085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A90" s="46" t="s">
         <v>136</v>
       </c>
@@ -8145,7 +8144,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A91" s="46" t="s">
         <v>142</v>
       </c>
@@ -8204,7 +8203,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A92" s="46" t="s">
         <v>144</v>
       </c>
@@ -8263,7 +8262,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A93" s="46" t="s">
         <v>146</v>
       </c>
@@ -8322,7 +8321,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A94" s="46" t="s">
         <v>148</v>
       </c>
@@ -8381,7 +8380,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A95" s="46" t="s">
         <v>150</v>
       </c>
@@ -8440,7 +8439,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A96" s="46" t="s">
         <v>178</v>
       </c>
@@ -8499,7 +8498,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A97" s="46" t="s">
         <v>180</v>
       </c>
@@ -8558,7 +8557,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A98" s="46" t="s">
         <v>181</v>
       </c>
@@ -8617,7 +8616,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A99" s="103">
         <v>6</v>
       </c>
@@ -8676,7 +8675,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A100" s="103">
         <v>7</v>
       </c>
@@ -8735,7 +8734,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A101" s="51"/>
       <c r="B101" s="52" t="s">
         <v>155</v>
@@ -8787,7 +8786,7 @@
         <v>21608839676161.926</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A102" s="104">
         <v>8</v>
       </c>
@@ -8843,7 +8842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A103" s="76"/>
       <c r="B103" s="74" t="s">
         <v>157</v>
@@ -8895,7 +8894,7 @@
         <v>21608839676161.926</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A104" s="14" t="s">
         <v>158</v>
       </c>
@@ -8919,7 +8918,7 @@
       <c r="S104" s="15"/>
       <c r="T104" s="15"/>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A105" s="14" t="s">
         <v>159</v>
       </c>
@@ -8943,59 +8942,59 @@
       <c r="S105" s="15"/>
       <c r="T105" s="15"/>
     </row>
-    <row r="107" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="107" t="s">
+    <row r="107" spans="1:22" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A107" s="128" t="s">
         <v>188</v>
       </c>
-      <c r="B107" s="108"/>
-      <c r="C107" s="108"/>
-      <c r="D107" s="108"/>
-      <c r="E107" s="108"/>
-      <c r="F107" s="108"/>
-      <c r="G107" s="108"/>
-      <c r="H107" s="108"/>
-      <c r="I107" s="109"/>
-      <c r="L107" s="107" t="s">
+      <c r="B107" s="129"/>
+      <c r="C107" s="129"/>
+      <c r="D107" s="129"/>
+      <c r="E107" s="129"/>
+      <c r="F107" s="129"/>
+      <c r="G107" s="129"/>
+      <c r="H107" s="129"/>
+      <c r="I107" s="130"/>
+      <c r="L107" s="128" t="s">
         <v>188</v>
       </c>
-      <c r="M107" s="108"/>
-      <c r="N107" s="108"/>
-      <c r="O107" s="108"/>
-      <c r="P107" s="108"/>
-      <c r="Q107" s="108"/>
-      <c r="R107" s="108"/>
-      <c r="S107" s="108"/>
-      <c r="T107" s="109"/>
-    </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A108" s="110" t="s">
+      <c r="M107" s="129"/>
+      <c r="N107" s="129"/>
+      <c r="O107" s="129"/>
+      <c r="P107" s="129"/>
+      <c r="Q107" s="129"/>
+      <c r="R107" s="129"/>
+      <c r="S107" s="129"/>
+      <c r="T107" s="130"/>
+    </row>
+    <row r="108" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A108" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B108" s="111"/>
-      <c r="C108" s="111"/>
-      <c r="D108" s="111"/>
-      <c r="E108" s="111"/>
-      <c r="F108" s="111"/>
-      <c r="G108" s="111"/>
-      <c r="H108" s="111"/>
-      <c r="I108" s="112"/>
-      <c r="L108" s="113" t="s">
+      <c r="B108" s="134"/>
+      <c r="C108" s="134"/>
+      <c r="D108" s="134"/>
+      <c r="E108" s="134"/>
+      <c r="F108" s="134"/>
+      <c r="G108" s="134"/>
+      <c r="H108" s="134"/>
+      <c r="I108" s="135"/>
+      <c r="L108" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="M108" s="111"/>
-      <c r="N108" s="111"/>
-      <c r="O108" s="111"/>
-      <c r="P108" s="111"/>
-      <c r="Q108" s="111"/>
-      <c r="R108" s="111"/>
-      <c r="S108" s="111"/>
-      <c r="T108" s="112"/>
-    </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A109" s="114" t="s">
+      <c r="M108" s="134"/>
+      <c r="N108" s="134"/>
+      <c r="O108" s="134"/>
+      <c r="P108" s="134"/>
+      <c r="Q108" s="134"/>
+      <c r="R108" s="134"/>
+      <c r="S108" s="134"/>
+      <c r="T108" s="135"/>
+    </row>
+    <row r="109" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A109" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="B109" s="115"/>
+      <c r="B109" s="123"/>
       <c r="C109" s="36" t="s">
         <v>126</v>
       </c>
@@ -9017,10 +9016,10 @@
       <c r="I109" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="L109" s="114" t="s">
+      <c r="L109" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="M109" s="115"/>
+      <c r="M109" s="123"/>
       <c r="N109" s="36" t="s">
         <v>126</v>
       </c>
@@ -9043,11 +9042,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A110" s="116">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A110" s="124">
         <v>-1</v>
       </c>
-      <c r="B110" s="117"/>
+      <c r="B110" s="125"/>
       <c r="C110" s="38">
         <v>-2</v>
       </c>
@@ -9069,10 +9068,10 @@
       <c r="I110" s="38">
         <v>-8</v>
       </c>
-      <c r="L110" s="116">
+      <c r="L110" s="124">
         <v>-1</v>
       </c>
-      <c r="M110" s="117"/>
+      <c r="M110" s="125"/>
       <c r="N110" s="38">
         <v>-2</v>
       </c>
@@ -9095,7 +9094,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A111" s="40">
         <v>1</v>
       </c>
@@ -9151,7 +9150,7 @@
         <v>23340202133015.043</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A112" s="71" t="s">
         <v>134</v>
       </c>
@@ -9207,7 +9206,7 @@
         <v>804204003832.31995</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A113" s="46" t="s">
         <v>136</v>
       </c>
@@ -9263,7 +9262,7 @@
         <v>22535998129182.715</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A114" s="46" t="s">
         <v>142</v>
       </c>
@@ -9319,7 +9318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A115" s="46" t="s">
         <v>144</v>
       </c>
@@ -9375,7 +9374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A116" s="103">
         <v>2</v>
       </c>
@@ -9434,7 +9433,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A117" s="103">
         <v>3</v>
       </c>
@@ -9490,7 +9489,7 @@
         <v>11649338812500.48</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A118" s="103">
         <v>4</v>
       </c>
@@ -9549,7 +9548,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A119" s="103">
         <v>5</v>
       </c>
@@ -9605,7 +9604,7 @@
         <v>87569473019857.906</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A120" s="71" t="s">
         <v>134</v>
       </c>
@@ -9664,7 +9663,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A121" s="46" t="s">
         <v>136</v>
       </c>
@@ -9723,7 +9722,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A122" s="46" t="s">
         <v>142</v>
       </c>
@@ -9782,7 +9781,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A123" s="46" t="s">
         <v>144</v>
       </c>
@@ -9841,7 +9840,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A124" s="46" t="s">
         <v>146</v>
       </c>
@@ -9900,7 +9899,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A125" s="46" t="s">
         <v>148</v>
       </c>
@@ -9959,7 +9958,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A126" s="46" t="s">
         <v>150</v>
       </c>
@@ -10018,7 +10017,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A127" s="46" t="s">
         <v>178</v>
       </c>
@@ -10077,7 +10076,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A128" s="46" t="s">
         <v>180</v>
       </c>
@@ -10136,7 +10135,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A129" s="46" t="s">
         <v>181</v>
       </c>
@@ -10195,7 +10194,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A130" s="46" t="s">
         <v>183</v>
       </c>
@@ -10254,7 +10253,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A131" s="103">
         <v>6</v>
       </c>
@@ -10313,7 +10312,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A132" s="103">
         <v>7</v>
       </c>
@@ -10372,7 +10371,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A133" s="51"/>
       <c r="B133" s="52" t="s">
         <v>155</v>
@@ -10424,8 +10423,8 @@
         <v>225231217221104.69</v>
       </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A134" s="120">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A134" s="131">
         <v>8</v>
       </c>
       <c r="B134" s="58" t="s">
@@ -10452,7 +10451,7 @@
       <c r="I134" s="70">
         <v>732.05</v>
       </c>
-      <c r="L134" s="120">
+      <c r="L134" s="131">
         <v>8</v>
       </c>
       <c r="M134" s="58" t="s">
@@ -10480,8 +10479,8 @@
         <v>27888088157529.598</v>
       </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A135" s="121"/>
+    <row r="135" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A135" s="132"/>
       <c r="B135" s="74" t="s">
         <v>157</v>
       </c>
@@ -10506,7 +10505,7 @@
       <c r="I135" s="75">
         <v>6644.27</v>
       </c>
-      <c r="L135" s="121"/>
+      <c r="L135" s="132"/>
       <c r="M135" s="74" t="s">
         <v>157</v>
       </c>
@@ -10532,7 +10531,7 @@
         <v>253119305378634.28</v>
       </c>
     </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A136" s="14" t="s">
         <v>193</v>
       </c>
@@ -10556,7 +10555,7 @@
       <c r="S136" s="15"/>
       <c r="T136" s="15"/>
     </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A137" s="15" t="s">
         <v>159</v>
       </c>
@@ -10580,59 +10579,59 @@
       <c r="S137" s="15"/>
       <c r="T137" s="15"/>
     </row>
-    <row r="139" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" s="107" t="s">
+    <row r="139" spans="1:22" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A139" s="128" t="s">
         <v>194</v>
       </c>
-      <c r="B139" s="108"/>
-      <c r="C139" s="108"/>
-      <c r="D139" s="108"/>
-      <c r="E139" s="108"/>
-      <c r="F139" s="108"/>
-      <c r="G139" s="108"/>
-      <c r="H139" s="108"/>
-      <c r="I139" s="109"/>
-      <c r="L139" s="107" t="s">
+      <c r="B139" s="129"/>
+      <c r="C139" s="129"/>
+      <c r="D139" s="129"/>
+      <c r="E139" s="129"/>
+      <c r="F139" s="129"/>
+      <c r="G139" s="129"/>
+      <c r="H139" s="129"/>
+      <c r="I139" s="130"/>
+      <c r="L139" s="128" t="s">
         <v>194</v>
       </c>
-      <c r="M139" s="108"/>
-      <c r="N139" s="108"/>
-      <c r="O139" s="108"/>
-      <c r="P139" s="108"/>
-      <c r="Q139" s="108"/>
-      <c r="R139" s="108"/>
-      <c r="S139" s="108"/>
-      <c r="T139" s="109"/>
-    </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A140" s="110" t="s">
+      <c r="M139" s="129"/>
+      <c r="N139" s="129"/>
+      <c r="O139" s="129"/>
+      <c r="P139" s="129"/>
+      <c r="Q139" s="129"/>
+      <c r="R139" s="129"/>
+      <c r="S139" s="129"/>
+      <c r="T139" s="130"/>
+    </row>
+    <row r="140" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A140" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B140" s="111"/>
-      <c r="C140" s="111"/>
-      <c r="D140" s="111"/>
-      <c r="E140" s="111"/>
-      <c r="F140" s="111"/>
-      <c r="G140" s="111"/>
-      <c r="H140" s="111"/>
-      <c r="I140" s="112"/>
-      <c r="L140" s="113" t="s">
+      <c r="B140" s="134"/>
+      <c r="C140" s="134"/>
+      <c r="D140" s="134"/>
+      <c r="E140" s="134"/>
+      <c r="F140" s="134"/>
+      <c r="G140" s="134"/>
+      <c r="H140" s="134"/>
+      <c r="I140" s="135"/>
+      <c r="L140" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="M140" s="111"/>
-      <c r="N140" s="111"/>
-      <c r="O140" s="111"/>
-      <c r="P140" s="111"/>
-      <c r="Q140" s="111"/>
-      <c r="R140" s="111"/>
-      <c r="S140" s="111"/>
-      <c r="T140" s="112"/>
-    </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A141" s="114" t="s">
+      <c r="M140" s="134"/>
+      <c r="N140" s="134"/>
+      <c r="O140" s="134"/>
+      <c r="P140" s="134"/>
+      <c r="Q140" s="134"/>
+      <c r="R140" s="134"/>
+      <c r="S140" s="134"/>
+      <c r="T140" s="135"/>
+    </row>
+    <row r="141" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A141" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="B141" s="115"/>
+      <c r="B141" s="123"/>
       <c r="C141" s="36" t="s">
         <v>126</v>
       </c>
@@ -10654,10 +10653,10 @@
       <c r="I141" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="L141" s="114" t="s">
+      <c r="L141" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="M141" s="115"/>
+      <c r="M141" s="123"/>
       <c r="N141" s="36" t="s">
         <v>126</v>
       </c>
@@ -10680,11 +10679,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A142" s="116">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A142" s="124">
         <v>-1</v>
       </c>
-      <c r="B142" s="117"/>
+      <c r="B142" s="125"/>
       <c r="C142" s="38">
         <v>-2</v>
       </c>
@@ -10706,10 +10705,10 @@
       <c r="I142" s="38">
         <v>-8</v>
       </c>
-      <c r="L142" s="116">
+      <c r="L142" s="124">
         <v>-1</v>
       </c>
-      <c r="M142" s="117"/>
+      <c r="M142" s="125"/>
       <c r="N142" s="38">
         <v>-2</v>
       </c>
@@ -10732,7 +10731,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A143" s="40">
         <v>1</v>
       </c>
@@ -10791,7 +10790,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A144" s="103">
         <v>2</v>
       </c>
@@ -10847,7 +10846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A145" s="103">
         <v>3</v>
       </c>
@@ -10906,7 +10905,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A146" s="103">
         <v>4</v>
       </c>
@@ -10962,7 +10961,7 @@
         <v>2048796367887.3601</v>
       </c>
     </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A147" s="71" t="s">
         <v>134</v>
       </c>
@@ -11021,7 +11020,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A148" s="46" t="s">
         <v>136</v>
       </c>
@@ -11080,7 +11079,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A149" s="46" t="s">
         <v>142</v>
       </c>
@@ -11139,7 +11138,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A150" s="46" t="s">
         <v>144</v>
       </c>
@@ -11198,7 +11197,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A151" s="46" t="s">
         <v>146</v>
       </c>
@@ -11257,7 +11256,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A152" s="46" t="s">
         <v>148</v>
       </c>
@@ -11316,7 +11315,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A153" s="46" t="s">
         <v>150</v>
       </c>
@@ -11375,7 +11374,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A154" s="46" t="s">
         <v>178</v>
       </c>
@@ -11434,7 +11433,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A155" s="46" t="s">
         <v>180</v>
       </c>
@@ -11493,7 +11492,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="156" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A156" s="46" t="s">
         <v>181</v>
       </c>
@@ -11552,7 +11551,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="157" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A157" s="103">
         <v>5</v>
       </c>
@@ -11611,7 +11610,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="158" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A158" s="103">
         <v>6</v>
       </c>
@@ -11667,7 +11666,7 @@
         <v>566485719421.44006</v>
       </c>
     </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A159" s="51"/>
       <c r="B159" s="52" t="s">
         <v>155</v>
@@ -11719,7 +11718,7 @@
         <v>4429407841098.2402</v>
       </c>
     </row>
-    <row r="160" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A160" s="104">
         <v>7</v>
       </c>
@@ -11775,7 +11774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A161" s="76"/>
       <c r="B161" s="74" t="s">
         <v>157</v>
@@ -11827,7 +11826,7 @@
         <v>4429407841098.2402</v>
       </c>
     </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A162" s="15"/>
       <c r="B162" s="78"/>
       <c r="C162" s="79"/>
@@ -11846,7 +11845,7 @@
       <c r="S162" s="80"/>
       <c r="T162" s="80"/>
     </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A163" s="14" t="s">
         <v>166</v>
       </c>
@@ -11870,7 +11869,7 @@
       <c r="S163" s="15"/>
       <c r="T163" s="15"/>
     </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A164" s="14" t="s">
         <v>159</v>
       </c>
@@ -11894,49 +11893,49 @@
       <c r="S164" s="15"/>
       <c r="T164" s="15"/>
     </row>
-    <row r="166" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A166" s="128" t="s">
+    <row r="166" spans="1:22" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A166" s="126" t="s">
         <v>196</v>
       </c>
-      <c r="B166" s="129"/>
-      <c r="C166" s="129"/>
-      <c r="D166" s="129"/>
-      <c r="E166" s="129"/>
-      <c r="F166" s="129"/>
-      <c r="G166" s="129"/>
-      <c r="H166" s="130"/>
-      <c r="L166" s="107" t="s">
+      <c r="B166" s="127"/>
+      <c r="C166" s="127"/>
+      <c r="D166" s="127"/>
+      <c r="E166" s="127"/>
+      <c r="F166" s="127"/>
+      <c r="G166" s="127"/>
+      <c r="H166" s="121"/>
+      <c r="L166" s="128" t="s">
         <v>196</v>
       </c>
-      <c r="M166" s="108"/>
-      <c r="N166" s="108"/>
-      <c r="O166" s="108"/>
-      <c r="P166" s="108"/>
-      <c r="Q166" s="108"/>
-      <c r="R166" s="109"/>
-    </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A167" s="131" t="s">
+      <c r="M166" s="129"/>
+      <c r="N166" s="129"/>
+      <c r="O166" s="129"/>
+      <c r="P166" s="129"/>
+      <c r="Q166" s="129"/>
+      <c r="R166" s="130"/>
+    </row>
+    <row r="167" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A167" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="B167" s="132"/>
-      <c r="C167" s="132"/>
-      <c r="D167" s="132"/>
-      <c r="E167" s="132"/>
-      <c r="F167" s="132"/>
-      <c r="G167" s="132"/>
-      <c r="H167" s="133"/>
-      <c r="L167" s="134" t="s">
+      <c r="B167" s="108"/>
+      <c r="C167" s="108"/>
+      <c r="D167" s="108"/>
+      <c r="E167" s="108"/>
+      <c r="F167" s="108"/>
+      <c r="G167" s="108"/>
+      <c r="H167" s="109"/>
+      <c r="L167" s="110" t="s">
         <v>101</v>
       </c>
-      <c r="M167" s="135"/>
-      <c r="N167" s="135"/>
-      <c r="O167" s="135"/>
-      <c r="P167" s="135"/>
-      <c r="Q167" s="135"/>
-      <c r="R167" s="136"/>
-    </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="M167" s="111"/>
+      <c r="N167" s="111"/>
+      <c r="O167" s="111"/>
+      <c r="P167" s="111"/>
+      <c r="Q167" s="111"/>
+      <c r="R167" s="112"/>
+    </row>
+    <row r="168" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A168" s="6" t="s">
         <v>110</v>
       </c>
@@ -11986,7 +11985,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A169" s="7">
         <v>-1</v>
       </c>
@@ -12036,29 +12035,29 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A170" s="137" t="s">
+    <row r="170" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A170" s="113" t="s">
         <v>197</v>
       </c>
-      <c r="B170" s="138"/>
-      <c r="C170" s="138"/>
-      <c r="D170" s="138"/>
-      <c r="E170" s="138"/>
-      <c r="F170" s="138"/>
-      <c r="G170" s="138"/>
-      <c r="H170" s="139"/>
-      <c r="L170" s="140" t="s">
+      <c r="B170" s="114"/>
+      <c r="C170" s="114"/>
+      <c r="D170" s="114"/>
+      <c r="E170" s="114"/>
+      <c r="F170" s="114"/>
+      <c r="G170" s="114"/>
+      <c r="H170" s="115"/>
+      <c r="L170" s="116" t="s">
         <v>197</v>
       </c>
-      <c r="M170" s="141"/>
-      <c r="N170" s="141"/>
-      <c r="O170" s="141"/>
-      <c r="P170" s="141"/>
-      <c r="Q170" s="141"/>
-      <c r="R170" s="141"/>
-      <c r="S170" s="142"/>
-    </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="M170" s="117"/>
+      <c r="N170" s="117"/>
+      <c r="O170" s="117"/>
+      <c r="P170" s="117"/>
+      <c r="Q170" s="117"/>
+      <c r="R170" s="117"/>
+      <c r="S170" s="118"/>
+    </row>
+    <row r="171" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A171" s="9" t="s">
         <v>25</v>
       </c>
@@ -12108,7 +12107,7 @@
         <v>433018440000000</v>
       </c>
     </row>
-    <row r="172" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A172" s="10" t="s">
         <v>26</v>
       </c>
@@ -12161,7 +12160,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A173" s="10" t="s">
         <v>27</v>
       </c>
@@ -12214,7 +12213,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="174" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A174" s="10" t="s">
         <v>28</v>
       </c>
@@ -12264,7 +12263,7 @@
         <v>21960000000</v>
       </c>
     </row>
-    <row r="175" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:22" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A175" s="86" t="s">
         <v>198</v>
       </c>
@@ -12317,7 +12316,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="176" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A176" s="10" t="s">
         <v>31</v>
       </c>
@@ -12370,7 +12369,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="177" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A177" s="11" t="s">
         <v>22</v>
       </c>
@@ -12423,7 +12422,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="178" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A178" s="10" t="s">
         <v>32</v>
       </c>
@@ -12476,7 +12475,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="179" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A179" s="12" t="s">
         <v>33</v>
       </c>
@@ -12529,7 +12528,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="180" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A180" s="13" t="s">
         <v>34</v>
       </c>
@@ -12579,29 +12578,29 @@
         <v>1154041560000000</v>
       </c>
     </row>
-    <row r="181" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A181" s="143" t="s">
+    <row r="181" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A181" s="119" t="s">
         <v>200</v>
       </c>
-      <c r="B181" s="144"/>
-      <c r="C181" s="144"/>
-      <c r="D181" s="144"/>
-      <c r="E181" s="144"/>
-      <c r="F181" s="144"/>
-      <c r="G181" s="144"/>
-      <c r="H181" s="130"/>
-      <c r="L181" s="143" t="s">
+      <c r="B181" s="120"/>
+      <c r="C181" s="120"/>
+      <c r="D181" s="120"/>
+      <c r="E181" s="120"/>
+      <c r="F181" s="120"/>
+      <c r="G181" s="120"/>
+      <c r="H181" s="121"/>
+      <c r="L181" s="119" t="s">
         <v>200</v>
       </c>
-      <c r="M181" s="144"/>
-      <c r="N181" s="144"/>
-      <c r="O181" s="144"/>
-      <c r="P181" s="144"/>
-      <c r="Q181" s="144"/>
-      <c r="R181" s="144"/>
-      <c r="S181" s="130"/>
-    </row>
-    <row r="182" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="M181" s="120"/>
+      <c r="N181" s="120"/>
+      <c r="O181" s="120"/>
+      <c r="P181" s="120"/>
+      <c r="Q181" s="120"/>
+      <c r="R181" s="120"/>
+      <c r="S181" s="121"/>
+    </row>
+    <row r="182" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A182" s="9" t="s">
         <v>35</v>
       </c>
@@ -12654,7 +12653,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="183" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A183" s="10" t="s">
         <v>36</v>
       </c>
@@ -12707,7 +12706,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="184" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A184" s="10" t="s">
         <v>37</v>
       </c>
@@ -12760,7 +12759,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="185" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A185" s="12" t="s">
         <v>38</v>
       </c>
@@ -12813,7 +12812,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="186" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A186" s="13" t="s">
         <v>39</v>
       </c>
@@ -12863,7 +12862,7 @@
         <v>747924480000000</v>
       </c>
     </row>
-    <row r="187" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A187" s="13" t="s">
         <v>40</v>
       </c>
@@ -12913,7 +12912,7 @@
         <v>1901966400000000</v>
       </c>
     </row>
-    <row r="188" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A188" s="13" t="s">
         <v>41</v>
       </c>
@@ -12963,7 +12962,7 @@
         <v>5211000000000</v>
       </c>
     </row>
-    <row r="189" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A189" s="14" t="s">
         <v>201</v>
       </c>
@@ -12983,7 +12982,7 @@
       <c r="Q189" s="15"/>
       <c r="R189" s="15"/>
     </row>
-    <row r="190" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A190" s="14" t="s">
         <v>202</v>
       </c>
@@ -13003,10 +13002,10 @@
       <c r="Q190" s="15"/>
       <c r="R190" s="15"/>
     </row>
-    <row r="191" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:22" x14ac:dyDescent="0.45">
       <c r="G191"/>
     </row>
-    <row r="192" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A192" s="93" t="s">
         <v>114</v>
       </c>
@@ -13020,7 +13019,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="193" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A193" s="105" t="s">
         <v>104</v>
       </c>
@@ -13047,7 +13046,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="194" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>99</v>
       </c>
@@ -13077,7 +13076,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="195" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>102</v>
       </c>
@@ -13100,7 +13099,7 @@
       <c r="L195" s="100"/>
       <c r="M195" s="101"/>
     </row>
-    <row r="196" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>112</v>
       </c>
@@ -13123,7 +13122,7 @@
       <c r="L196" s="100"/>
       <c r="M196" s="101"/>
     </row>
-    <row r="197" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>97</v>
       </c>
@@ -13146,7 +13145,7 @@
       <c r="L197" s="100"/>
       <c r="M197" s="101"/>
     </row>
-    <row r="198" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>95</v>
       </c>
@@ -13169,7 +13168,7 @@
       <c r="L198" s="100"/>
       <c r="M198" s="101"/>
     </row>
-    <row r="199" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>113</v>
       </c>
@@ -13191,7 +13190,7 @@
       <c r="L199" s="100"/>
       <c r="M199" s="101"/>
     </row>
-    <row r="200" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>94</v>
       </c>
@@ -13213,7 +13212,7 @@
       <c r="L200" s="100"/>
       <c r="M200" s="101"/>
     </row>
-    <row r="201" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A201" s="105" t="s">
         <v>93</v>
       </c>
@@ -13237,72 +13236,72 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L1:T1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="L2:T2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="L29:T29"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="L30:T30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="A44:I44"/>
+    <mergeCell ref="L44:T44"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="L45:T45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="L71:L72"/>
+    <mergeCell ref="A76:I76"/>
+    <mergeCell ref="L76:T76"/>
+    <mergeCell ref="A77:I77"/>
+    <mergeCell ref="L77:T77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="L78:M78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="L79:M79"/>
+    <mergeCell ref="A80:I80"/>
+    <mergeCell ref="L80:T80"/>
+    <mergeCell ref="A107:I107"/>
+    <mergeCell ref="L107:T107"/>
+    <mergeCell ref="A108:I108"/>
+    <mergeCell ref="L108:T108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="L109:M109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="L110:M110"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="L134:L135"/>
+    <mergeCell ref="A139:I139"/>
+    <mergeCell ref="L139:T139"/>
+    <mergeCell ref="A140:I140"/>
+    <mergeCell ref="L140:T140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="L141:M141"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="L142:M142"/>
+    <mergeCell ref="A166:H166"/>
+    <mergeCell ref="L166:R166"/>
     <mergeCell ref="A167:H167"/>
     <mergeCell ref="L167:R167"/>
     <mergeCell ref="A170:H170"/>
     <mergeCell ref="L170:S170"/>
     <mergeCell ref="A181:H181"/>
     <mergeCell ref="L181:S181"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="L141:M141"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="L142:M142"/>
-    <mergeCell ref="A166:H166"/>
-    <mergeCell ref="L166:R166"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="L134:L135"/>
-    <mergeCell ref="A139:I139"/>
-    <mergeCell ref="L139:T139"/>
-    <mergeCell ref="A140:I140"/>
-    <mergeCell ref="L140:T140"/>
-    <mergeCell ref="A108:I108"/>
-    <mergeCell ref="L108:T108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="L109:M109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="L110:M110"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="L79:M79"/>
-    <mergeCell ref="A80:I80"/>
-    <mergeCell ref="L80:T80"/>
-    <mergeCell ref="A107:I107"/>
-    <mergeCell ref="L107:T107"/>
-    <mergeCell ref="A76:I76"/>
-    <mergeCell ref="L76:T76"/>
-    <mergeCell ref="A77:I77"/>
-    <mergeCell ref="L77:T77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="L78:M78"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="A44:I44"/>
-    <mergeCell ref="L44:T44"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="L45:T45"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="L30:T30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="L29:T29"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L1:T1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="L2:T2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13310,29 +13309,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.1328125" customWidth="1"/>
+    <col min="2" max="2" width="35.59765625" customWidth="1"/>
+    <col min="4" max="4" width="6.1328125" customWidth="1"/>
+    <col min="5" max="5" width="31.1328125" customWidth="1"/>
+    <col min="7" max="7" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.3984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -13370,7 +13369,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -13385,8 +13384,8 @@
         <v>1</v>
       </c>
       <c r="G2" s="102">
-        <f>$B$2/100</f>
-        <v>9.3451624089700615E-3</v>
+        <f>$B$2</f>
+        <v>0.93451624089700613</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -13413,7 +13412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -13428,8 +13427,8 @@
         <v>1</v>
       </c>
       <c r="G3" s="102">
-        <f t="shared" ref="G3:G9" si="0">$B$2/100</f>
-        <v>9.3451624089700615E-3</v>
+        <f t="shared" ref="G3:G9" si="0">$B$2</f>
+        <v>0.93451624089700613</v>
       </c>
       <c r="H3">
         <f>SUM(B20:B21)/SUM(B20:B21,B25:B28)</f>
@@ -13457,7 +13456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -13472,7 +13471,7 @@
       </c>
       <c r="G4" s="102">
         <f t="shared" si="0"/>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -13499,7 +13498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E5" s="33" t="s">
         <v>85</v>
       </c>
@@ -13508,7 +13507,7 @@
       </c>
       <c r="G5" s="102">
         <f t="shared" si="0"/>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -13535,7 +13534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="E6" s="33" t="s">
         <v>86</v>
       </c>
@@ -13544,7 +13543,7 @@
       </c>
       <c r="G6" s="102">
         <f t="shared" si="0"/>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -13571,7 +13570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -13584,7 +13583,7 @@
       </c>
       <c r="G7" s="102">
         <f t="shared" si="0"/>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -13611,11 +13610,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="107" t="s">
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A8" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="108"/>
+      <c r="B8" s="129"/>
       <c r="E8" s="33" t="s">
         <v>88</v>
       </c>
@@ -13624,7 +13623,7 @@
       </c>
       <c r="G8" s="102">
         <f t="shared" si="0"/>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -13651,11 +13650,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="134" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="135"/>
+      <c r="B9" s="111"/>
       <c r="E9" s="33" t="s">
         <v>89</v>
       </c>
@@ -13664,7 +13663,7 @@
       </c>
       <c r="G9" s="102">
         <f t="shared" si="0"/>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="H9">
         <f>SUM(B14:B15,B17,B19,B22)/SUM(B14:B15,B17, B19,B22,B25:B28)</f>
@@ -13692,7 +13691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
@@ -13700,7 +13699,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>-1</v>
       </c>
@@ -13708,13 +13707,13 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="145" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="146"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>25</v>
       </c>
@@ -13722,7 +13721,7 @@
         <v>12028.3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
         <v>26</v>
       </c>
@@ -13734,7 +13733,7 @@
         <v>Other</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
         <v>27</v>
       </c>
@@ -13746,7 +13745,7 @@
         <v>Other</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
         <v>28</v>
       </c>
@@ -13754,7 +13753,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>29</v>
       </c>
@@ -13766,13 +13765,13 @@
         <v>Other</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="25"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
         <v>31</v>
       </c>
@@ -13784,7 +13783,7 @@
         <v>Other</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>22</v>
       </c>
@@ -13796,7 +13795,7 @@
         <v>Natural Gas and Petroleum Systems</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
         <v>32</v>
       </c>
@@ -13808,7 +13807,7 @@
         <v>Natural Gas and Petroleum Systems</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>33</v>
       </c>
@@ -13820,7 +13819,7 @@
         <v>Other</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="13" t="s">
         <v>34</v>
       </c>
@@ -13829,13 +13828,13 @@
         <v>32056.83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="145" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="146"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>35</v>
       </c>
@@ -13843,7 +13842,7 @@
         <v>14675.67</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>36</v>
       </c>
@@ -13851,7 +13850,7 @@
         <v>4024.13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="10" t="s">
         <v>37</v>
       </c>
@@ -13859,7 +13858,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>38</v>
       </c>
@@ -13867,7 +13866,7 @@
         <v>797.87</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="13" t="s">
         <v>39</v>
       </c>
@@ -13876,7 +13875,7 @@
         <v>20775.669999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="13" t="s">
         <v>40</v>
       </c>
@@ -13885,7 +13884,7 @@
         <v>52832.5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
         <v>41</v>
       </c>
@@ -13894,42 +13893,42 @@
         <v>144.74657534246575</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>67</v>
       </c>
       <c r="B33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="27" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="17" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B37" s="15"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="18" t="s">
         <v>42</v>
       </c>
@@ -13937,7 +13936,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="19" t="s">
         <v>43</v>
       </c>
@@ -13945,7 +13944,7 @@
         <v>11.33</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="19" t="s">
         <v>44</v>
       </c>
@@ -13953,7 +13952,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="19" t="s">
         <v>45</v>
       </c>
@@ -13962,7 +13961,7 @@
         <v>58.33</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="18" t="s">
         <v>46</v>
       </c>
@@ -13973,7 +13972,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="19" t="s">
         <v>47</v>
       </c>
@@ -13982,7 +13981,7 @@
       </c>
       <c r="C43" s="29"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="19" t="s">
         <v>48</v>
       </c>
@@ -13991,7 +13990,7 @@
       </c>
       <c r="C44" s="29"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="19" t="s">
         <v>49</v>
       </c>
@@ -14000,7 +13999,7 @@
       </c>
       <c r="C45" s="29"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="19" t="s">
         <v>50</v>
       </c>
@@ -14009,7 +14008,7 @@
       </c>
       <c r="C46" s="29"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="19" t="s">
         <v>51</v>
       </c>
@@ -14018,7 +14017,7 @@
       </c>
       <c r="C47" s="29"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="19" t="s">
         <v>52</v>
       </c>
@@ -14027,7 +14026,7 @@
       </c>
       <c r="C48" s="29"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="18" t="s">
         <v>53</v>
       </c>
@@ -14039,7 +14038,7 @@
         <v>161.27000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="18" t="s">
         <v>54</v>
       </c>
@@ -14048,19 +14047,19 @@
         <v>897.34000000000015</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B51" s="31"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B52" s="31"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -14069,7 +14068,7 @@
         <v>11.33</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -14078,7 +14077,7 @@
         <v>173.02</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>120</v>
       </c>
@@ -14100,23 +14099,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="32" t="s">
         <v>77</v>
       </c>
@@ -14151,7 +14150,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="33" t="s">
         <v>82</v>
       </c>
@@ -14161,7 +14160,7 @@
       </c>
       <c r="C2" s="34">
         <f>Calcs!G2</f>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="D2" s="34">
         <f>Calcs!H2</f>
@@ -14196,7 +14195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="33" t="s">
         <v>83</v>
       </c>
@@ -14206,7 +14205,7 @@
       </c>
       <c r="C3" s="34">
         <f>Calcs!G3</f>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="D3" s="34">
         <f>Calcs!H3</f>
@@ -14241,7 +14240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="33" t="s">
         <v>84</v>
       </c>
@@ -14251,7 +14250,7 @@
       </c>
       <c r="C4" s="34">
         <f>Calcs!G4</f>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="D4" s="34">
         <f>Calcs!H4</f>
@@ -14286,7 +14285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="33" t="s">
         <v>85</v>
       </c>
@@ -14296,7 +14295,7 @@
       </c>
       <c r="C5" s="34">
         <f>Calcs!G5</f>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="D5" s="34">
         <f>Calcs!H5</f>
@@ -14331,7 +14330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="33" t="s">
         <v>86</v>
       </c>
@@ -14341,7 +14340,7 @@
       </c>
       <c r="C6" s="34">
         <f>Calcs!G6</f>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="D6" s="34">
         <f>Calcs!H6</f>
@@ -14376,7 +14375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="33" t="s">
         <v>87</v>
       </c>
@@ -14386,7 +14385,7 @@
       </c>
       <c r="C7" s="34">
         <f>Calcs!G7</f>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="D7" s="34">
         <f>Calcs!H7</f>
@@ -14421,7 +14420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="33" t="s">
         <v>88</v>
       </c>
@@ -14431,7 +14430,7 @@
       </c>
       <c r="C8" s="34">
         <f>Calcs!G8</f>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="D8" s="34">
         <f>Calcs!H8</f>
@@ -14466,7 +14465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="33" t="s">
         <v>89</v>
       </c>
@@ -14476,7 +14475,7 @@
       </c>
       <c r="C9" s="34">
         <f>Calcs!G9</f>
-        <v>9.3451624089700615E-3</v>
+        <v>0.93451624089700613</v>
       </c>
       <c r="D9" s="34">
         <f>Calcs!H9</f>

</xml_diff>

<commit_message>
Industry fuel consumption updates
</commit_message>
<xml_diff>
--- a/InputData/indst/BPoIFUfE/BAU Proportion of Industrial Fuel Used for Energy.xlsx
+++ b/InputData/indst/BPoIFUfE/BAU Proportion of Industrial Fuel Used for Energy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\indst\BPoIFUfE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1B90FC-77E1-42B9-9829-B96B2B78BF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B3C99E-BB06-4E1E-BFF5-8137F70E9330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3289,17 +3289,17 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="2" max="2" width="58.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3307,132 +3307,132 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>2021</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -3454,18 +3454,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="2" max="33" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>2973748362467874.5</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>7765601358445139</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>374268033031227.38</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>677857735918.88794</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>1563545743104663.8</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -4408,7 +4408,7 @@
       <c r="AF12" s="34"/>
       <c r="AG12" s="34"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
@@ -4459,20 +4459,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="29" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="2" max="29" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>716594579368250.75</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>134246378456019.61</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>935103830040788.88</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>329978016927545.25</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
@@ -5429,14 +5429,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="27"/>
       <c r="B1" s="40" t="s">
         <v>90</v>
@@ -5446,7 +5446,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="27"/>
       <c r="B2" s="27" t="s">
         <v>92</v>
@@ -5455,7 +5455,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>94</v>
       </c>
@@ -5466,12 +5466,12 @@
         <v>14262</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>239000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
         <v>98</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>3616.0720537220332</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>14340.148461283854</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>14340148.461283853</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3.9656699999999998</v>
       </c>
@@ -5545,22 +5545,22 @@
       <selection activeCell="A25" sqref="A25:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.1796875" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="4" max="4" width="6.1796875" customWidth="1"/>
+    <col min="5" max="5" width="31.1796875" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -5568,7 +5568,7 @@
       <c r="E1" s="24"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>17</v>
       </c>
@@ -5576,7 +5576,7 @@
       <c r="E2" s="24"/>
       <c r="G2" s="28"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="43" t="s">
         <v>37</v>
       </c>
@@ -5584,7 +5584,7 @@
       <c r="E3" s="24"/>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>-1</v>
       </c>
@@ -5600,13 +5600,13 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="45" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="46"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>23</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>12005</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>69</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
         <v>70</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>9206</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>7047</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>31</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>26</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>3393</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>27</v>
       </c>
@@ -5679,13 +5679,13 @@
         <v>34344</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="45" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="46"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>29</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>30</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>32</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>19497</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>33</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>53841</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
@@ -5745,28 +5745,28 @@
         <v>147.50958904109589</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="14"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="21"/>
       <c r="B24" s="14"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -5824,12 +5824,12 @@
         <v>257.44</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>2.97</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>66</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>354.79000000000008</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>0.53826797488169997</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="39" t="s">
         <v>103</v>
       </c>
@@ -5916,16 +5916,16 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>39</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>44</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="24" t="s">
         <v>45</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
         <v>46</v>
       </c>
@@ -6038,8 +6038,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="25">
-        <f>1-Calcs!B36</f>
-        <v>0.66146886504594438</v>
+        <v>1</v>
       </c>
       <c r="D4" s="25">
         <v>0</v>
@@ -6066,7 +6065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
         <v>47</v>
       </c>
@@ -6101,7 +6100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
         <v>48</v>
       </c>
@@ -6136,7 +6135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>49</v>
       </c>
@@ -6171,7 +6170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
         <v>50</v>
       </c>
@@ -6206,7 +6205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
         <v>51</v>
       </c>

</xml_diff>